<commit_message>
small debugs + dataset comparison added. bench complete. DFSnLogic still unsatisfactory
</commit_message>
<xml_diff>
--- a/testing/statistics/DFSnLogicBench.xlsx
+++ b/testing/statistics/DFSnLogicBench.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fuux\Desktop\Nonograms\OfficialGitRepo\nonogram\testing\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1DDCE4-A1F5-4911-967E-6BA057D8A996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E680C4D0-07BC-42E7-A02D-242139998AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1320" yWindow="5220" windowWidth="28725" windowHeight="11520" xr2:uid="{5789A875-4E7B-4190-9FD4-8CA15800E325}"/>
+    <workbookView xWindow="-4785" yWindow="1980" windowWidth="28725" windowHeight="11520" xr2:uid="{5789A875-4E7B-4190-9FD4-8CA15800E325}"/>
   </bookViews>
   <sheets>
     <sheet name="DFSBenchmarkSmall" sheetId="2" r:id="rId1"/>
@@ -2702,8 +2702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE03B4F-9C31-4132-8F18-C8C1B1757BAA}">
   <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y29" sqref="Y29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3659,7 +3659,7 @@
         <v>5.4738366051685161E-6</v>
       </c>
       <c r="X19">
-        <f>R19 *200</f>
+        <f t="shared" ref="X19:X41" si="1">R19 *200</f>
         <v>1.0947673210337032E-5</v>
       </c>
     </row>
@@ -3668,7 +3668,7 @@
         <v>5</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:C32" si="1">B20*B20</f>
+        <f t="shared" ref="C20:C32" si="2">B20*B20</f>
         <v>25</v>
       </c>
       <c r="D20" s="2">
@@ -3678,15 +3678,15 @@
         <v>5</v>
       </c>
       <c r="O20">
-        <f t="shared" ref="O20:O49" si="2">N20*N20</f>
+        <f t="shared" ref="O20:O49" si="3">N20*N20</f>
         <v>25</v>
       </c>
       <c r="P20">
-        <f t="shared" ref="P20:P49" si="3">94.396*POWER(EXP(1), (0.046*O20))</f>
+        <f t="shared" ref="P20:P49" si="4">94.396*POWER(EXP(1), (0.046*O20))</f>
         <v>298.12077790307529</v>
       </c>
       <c r="Q20">
-        <f t="shared" ref="Q20:Q49" si="4">(P20/(1000000*60))</f>
+        <f t="shared" ref="Q20:Q49" si="5">(P20/(1000000*60))</f>
         <v>4.9686796317179213E-6</v>
       </c>
       <c r="R20">
@@ -3694,23 +3694,23 @@
         <v>8.2811327195298687E-8</v>
       </c>
       <c r="S20">
-        <f t="shared" ref="S20:S49" si="5">R20/24</f>
+        <f t="shared" ref="S20:S49" si="6">R20/24</f>
         <v>3.4504719664707788E-9</v>
       </c>
       <c r="T20">
-        <f t="shared" ref="T20:T49" si="6">S20/365</f>
+        <f t="shared" ref="T20:T49" si="7">S20/365</f>
         <v>9.4533478533445989E-12</v>
       </c>
       <c r="V20">
-        <f t="shared" ref="V20:V41" si="7">R20*52</f>
+        <f t="shared" ref="V20:V41" si="8">R20*52</f>
         <v>4.3061890141555319E-6</v>
       </c>
       <c r="W20">
-        <f t="shared" ref="W20:W41" si="8">R20*100</f>
+        <f t="shared" ref="W20:W41" si="9">R20*100</f>
         <v>8.2811327195298691E-6</v>
       </c>
       <c r="X20">
-        <f>R20 *200</f>
+        <f t="shared" si="1"/>
         <v>1.6562265439059738E-5</v>
       </c>
     </row>
@@ -3719,7 +3719,7 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="D21" s="1">
@@ -3729,15 +3729,15 @@
         <v>6</v>
       </c>
       <c r="O21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="P21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>494.47604121951184</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.2412673536585307E-6</v>
       </c>
       <c r="R21">
@@ -3745,23 +3745,23 @@
         <v>1.3735445589430886E-7</v>
       </c>
       <c r="S21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.7231023289295357E-9</v>
       </c>
       <c r="T21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.5679732408026125E-11</v>
       </c>
       <c r="V21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.1424317065040609E-6</v>
       </c>
       <c r="W21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.3735445589430886E-5</v>
       </c>
       <c r="X21">
-        <f>R21 *200</f>
+        <f t="shared" si="1"/>
         <v>2.7470891178861771E-5</v>
       </c>
     </row>
@@ -3770,7 +3770,7 @@
         <v>7</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="D22" s="2">
@@ -3780,15 +3780,15 @@
         <v>7</v>
       </c>
       <c r="O22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="P22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>899.19390365410447</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.4986565060901741E-5</v>
       </c>
       <c r="R22">
@@ -3796,23 +3796,23 @@
         <v>2.4977608434836235E-7</v>
       </c>
       <c r="S22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0407336847848431E-8</v>
       </c>
       <c r="T22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.8513251637940907E-11</v>
       </c>
       <c r="V22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2988356386114842E-5</v>
       </c>
       <c r="W22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.4977608434836234E-5</v>
       </c>
       <c r="X22">
-        <f>R22 *200</f>
+        <f t="shared" si="1"/>
         <v>4.9955216869672467E-5</v>
       </c>
     </row>
@@ -3821,7 +3821,7 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="D23" s="1">
@@ -3831,15 +3831,15 @@
         <v>8</v>
       </c>
       <c r="O23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="P23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1792.7368531126717</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.987894755187786E-5</v>
       </c>
       <c r="R23">
@@ -3847,23 +3847,23 @@
         <v>4.9798245919796435E-7</v>
       </c>
       <c r="S23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.0749269133248516E-8</v>
       </c>
       <c r="T23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.6847312693831552E-11</v>
       </c>
       <c r="V23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.5895087878294145E-5</v>
       </c>
       <c r="W23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.9798245919796435E-5</v>
       </c>
       <c r="X23">
-        <f>R23 *200</f>
+        <f t="shared" si="1"/>
         <v>9.959649183959287E-5</v>
       </c>
     </row>
@@ -3872,7 +3872,7 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="D24" s="2">
@@ -3882,15 +3882,15 @@
         <v>9</v>
       </c>
       <c r="O24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="P24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3918.6351626790838</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.5310586044651402E-5</v>
       </c>
       <c r="R24">
@@ -3898,23 +3898,23 @@
         <v>1.0885097674108565E-6</v>
       </c>
       <c r="S24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5354573642119019E-8</v>
       </c>
       <c r="T24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.2425910586881924E-10</v>
       </c>
       <c r="V24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.660250790536454E-5</v>
       </c>
       <c r="W24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.0885097674108565E-4</v>
       </c>
       <c r="X24">
-        <f>R24 *200</f>
+        <f t="shared" si="1"/>
         <v>2.177019534821713E-4</v>
       </c>
     </row>
@@ -3923,7 +3923,7 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="D25" s="1">
@@ -3933,15 +3933,15 @@
         <v>10</v>
       </c>
       <c r="O25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="P25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9390.9214593359811</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5651535765559969E-4</v>
       </c>
       <c r="R25">
@@ -3949,23 +3949,23 @@
         <v>2.6085892942599949E-6</v>
       </c>
       <c r="S25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0869122059416645E-7</v>
       </c>
       <c r="T25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.977841660114149E-10</v>
       </c>
       <c r="V25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.3564664330151973E-4</v>
       </c>
       <c r="W25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.6085892942599948E-4</v>
       </c>
       <c r="X25">
-        <f>R25 *200</f>
+        <f t="shared" si="1"/>
         <v>5.2171785885199895E-4</v>
       </c>
     </row>
@@ -3974,7 +3974,7 @@
         <v>11</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="D26" s="2">
@@ -3984,15 +3984,15 @@
         <v>11</v>
       </c>
       <c r="O26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="P26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24673.836232813268</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.1123060388022112E-4</v>
       </c>
       <c r="R26">
@@ -4000,23 +4000,23 @@
         <v>6.8538433980036859E-6</v>
       </c>
       <c r="S26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.8557680825015356E-7</v>
       </c>
       <c r="T26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.8240221438398231E-10</v>
       </c>
       <c r="V26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.5639985669619166E-4</v>
       </c>
       <c r="W26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.8538433980036854E-4</v>
       </c>
       <c r="X26">
-        <f>R26 *200</f>
+        <f t="shared" si="1"/>
         <v>1.3707686796007371E-3</v>
       </c>
     </row>
@@ -4025,7 +4025,7 @@
         <v>12</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="D27" s="1">
@@ -4035,15 +4035,15 @@
         <v>12</v>
       </c>
       <c r="O27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>144</v>
       </c>
       <c r="P27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>71075.551746928657</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1845925291154777E-3</v>
       </c>
       <c r="R27">
@@ -4051,23 +4051,23 @@
         <v>1.9743208818591295E-5</v>
       </c>
       <c r="S27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.2263370077463728E-7</v>
       </c>
       <c r="T27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.2537909610264034E-9</v>
       </c>
       <c r="V27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0266468585667474E-3</v>
       </c>
       <c r="W27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.9743208818591295E-3</v>
       </c>
       <c r="X27">
-        <f>R27 *200</f>
+        <f t="shared" si="1"/>
         <v>3.9486417637182589E-3</v>
       </c>
     </row>
@@ -4076,7 +4076,7 @@
         <v>13</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="D28" s="2">
@@ -4086,15 +4086,15 @@
         <v>13</v>
       </c>
       <c r="O28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>169</v>
       </c>
       <c r="P28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>224470.3035794383</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.7411717263239716E-3</v>
       </c>
       <c r="R28">
@@ -4102,23 +4102,23 @@
         <v>6.2352862105399535E-5</v>
       </c>
       <c r="S28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.5980359210583141E-6</v>
       </c>
       <c r="T28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.1179066330364766E-9</v>
       </c>
       <c r="V28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.2423488294807757E-3</v>
       </c>
       <c r="W28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2352862105399531E-3</v>
       </c>
       <c r="X28">
-        <f>R28 *200</f>
+        <f t="shared" si="1"/>
         <v>1.2470572421079906E-2</v>
       </c>
     </row>
@@ -4127,7 +4127,7 @@
         <v>14</v>
       </c>
       <c r="C29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
       <c r="D29" s="1">
@@ -4137,15 +4137,15 @@
         <v>14</v>
       </c>
       <c r="O29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>196</v>
       </c>
       <c r="P29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>777235.52109541721</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2953925351590286E-2</v>
       </c>
       <c r="R29">
@@ -4153,23 +4153,23 @@
         <v>2.1589875585983811E-4</v>
       </c>
       <c r="S29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.9957814941599218E-6</v>
       </c>
       <c r="T29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4645976696328554E-8</v>
       </c>
       <c r="V29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1226735304711582E-2</v>
       </c>
       <c r="W29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.1589875585983812E-2</v>
       </c>
       <c r="X29">
-        <f>R29 *200</f>
+        <f t="shared" si="1"/>
         <v>4.3179751171967623E-2</v>
       </c>
     </row>
@@ -4178,7 +4178,7 @@
         <v>15</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
       <c r="D30" s="2">
@@ -4188,15 +4188,15 @@
         <v>15</v>
       </c>
       <c r="O30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>225</v>
       </c>
       <c r="P30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2950539.8139998666</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.9175663566664446E-2</v>
       </c>
       <c r="R30">
@@ -4204,23 +4204,23 @@
         <v>8.1959439277774077E-4</v>
       </c>
       <c r="S30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.4149766365739201E-5</v>
       </c>
       <c r="T30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.3561003741751236E-8</v>
       </c>
       <c r="V30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.261890842444252E-2</v>
       </c>
       <c r="W30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.1959439277774077E-2</v>
       </c>
       <c r="X30">
-        <f>R30 *200</f>
+        <f t="shared" si="1"/>
         <v>0.16391887855554815</v>
       </c>
     </row>
@@ -4229,7 +4229,7 @@
         <v>16</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
       <c r="D31" s="1">
@@ -4239,15 +4239,15 @@
         <v>16</v>
       </c>
       <c r="O31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>256</v>
       </c>
       <c r="P31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12280199.16711692</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.20466998611861534</v>
       </c>
       <c r="R31">
@@ -4255,23 +4255,23 @@
         <v>3.4111664353102555E-3</v>
       </c>
       <c r="S31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4213193480459399E-4</v>
       </c>
       <c r="T31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.8940256110847666E-7</v>
       </c>
       <c r="V31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.17738065463613328</v>
       </c>
       <c r="W31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.34111664353102555</v>
       </c>
       <c r="X31">
-        <f>R31 *200</f>
+        <f t="shared" si="1"/>
         <v>0.68223328706205111</v>
       </c>
     </row>
@@ -4280,7 +4280,7 @@
         <v>17</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>289</v>
       </c>
       <c r="D32" s="2">
@@ -4290,15 +4290,15 @@
         <v>17</v>
       </c>
       <c r="O32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>289</v>
       </c>
       <c r="P32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>56035652.582034968</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.93392754303391612</v>
       </c>
       <c r="R32">
@@ -4306,23 +4306,23 @@
         <v>1.5565459050565269E-2</v>
       </c>
       <c r="S32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.4856079377355292E-4</v>
       </c>
       <c r="T32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7768788870508299E-6</v>
       </c>
       <c r="V32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.80940387062939401</v>
       </c>
       <c r="W32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.5565459050565269</v>
       </c>
       <c r="X32">
-        <f>R32 *200</f>
+        <f t="shared" si="1"/>
         <v>3.1130918101130538</v>
       </c>
     </row>
@@ -4331,15 +4331,15 @@
         <v>18</v>
       </c>
       <c r="O33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>324</v>
       </c>
       <c r="P33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>280335791.89638656</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.6722631982731091</v>
       </c>
       <c r="R33">
@@ -4347,23 +4347,23 @@
         <v>7.7871053304551824E-2</v>
       </c>
       <c r="S33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2446272210229928E-3</v>
       </c>
       <c r="T33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.8893896466383366E-6</v>
       </c>
       <c r="V33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.0492947718366947</v>
       </c>
       <c r="W33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7.7871053304551827</v>
       </c>
       <c r="X33">
-        <f>R33 *200</f>
+        <f t="shared" si="1"/>
         <v>15.574210660910365</v>
       </c>
     </row>
@@ -4372,15 +4372,15 @@
         <v>19</v>
       </c>
       <c r="O34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>361</v>
       </c>
       <c r="P34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1537615534.7465544</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>25.626925579109241</v>
       </c>
       <c r="R34">
@@ -4388,23 +4388,23 @@
         <v>0.42711542631848731</v>
       </c>
       <c r="S34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.7796476096603637E-2</v>
       </c>
       <c r="T34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.875746875781818E-5</v>
       </c>
       <c r="V34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>22.210002168561338</v>
       </c>
       <c r="W34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>42.711542631848729</v>
       </c>
       <c r="X34">
-        <f>R34 *200</f>
+        <f t="shared" si="1"/>
         <v>85.423085263697459</v>
       </c>
     </row>
@@ -4413,15 +4413,15 @@
         <v>20</v>
       </c>
       <c r="O35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>400</v>
       </c>
       <c r="P35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9246386831.6984615</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>154.10644719497435</v>
       </c>
       <c r="R35">
@@ -4429,23 +4429,23 @@
         <v>2.5684407865829062</v>
       </c>
       <c r="S35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.1070183661076211</v>
       </c>
       <c r="T35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.9320100303457833E-4</v>
       </c>
       <c r="V35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>133.55892090231112</v>
       </c>
       <c r="W35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>256.84407865829064</v>
       </c>
       <c r="X35">
-        <f>R35 *200</f>
+        <f t="shared" si="1"/>
         <v>513.68815731658128</v>
       </c>
     </row>
@@ -4454,15 +4454,15 @@
         <v>21</v>
       </c>
       <c r="O36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>441</v>
       </c>
       <c r="P36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60960911422.671539</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1016.015190377859</v>
       </c>
       <c r="R36">
@@ -4470,23 +4470,23 @@
         <v>16.933586506297651</v>
       </c>
       <c r="S36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.70556610442906875</v>
       </c>
       <c r="T36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.9330578203536131E-3</v>
       </c>
       <c r="V36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>880.54649832747782</v>
       </c>
       <c r="W36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1693.3586506297652</v>
       </c>
       <c r="X36">
-        <f>R36 *200</f>
+        <f t="shared" si="1"/>
         <v>3386.7173012595304</v>
       </c>
     </row>
@@ -4495,7 +4495,7 @@
         <v>22</v>
       </c>
       <c r="O37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>484</v>
       </c>
       <c r="P37">
@@ -4503,7 +4503,7 @@
         <v>440642047608.44647</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7344.0341268074408</v>
       </c>
       <c r="R37">
@@ -4511,23 +4511,23 @@
         <v>122.40056878012402</v>
       </c>
       <c r="S37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.1000236991718344</v>
       </c>
       <c r="T37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.3972667668963931E-2</v>
       </c>
       <c r="V37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6364.8295765664488</v>
       </c>
       <c r="W37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>12240.056878012401</v>
       </c>
       <c r="X37">
-        <f>R37 *200</f>
+        <f t="shared" si="1"/>
         <v>24480.113756024803</v>
       </c>
     </row>
@@ -4536,15 +4536,15 @@
         <v>23</v>
       </c>
       <c r="O38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>529</v>
       </c>
       <c r="P38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3492010285583.9521</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>58200.171426399203</v>
       </c>
       <c r="R38">
@@ -4556,19 +4556,19 @@
         <v>40.416785712777219</v>
       </c>
       <c r="T38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.11073091976103348</v>
       </c>
       <c r="V38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50440.148569545971</v>
       </c>
       <c r="W38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>97000.285710665339</v>
       </c>
       <c r="X38">
-        <f>R38 *200</f>
+        <f t="shared" si="1"/>
         <v>194000.57142133068</v>
       </c>
     </row>
@@ -4577,15 +4577,15 @@
         <v>24</v>
       </c>
       <c r="O39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>576</v>
       </c>
       <c r="P39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30340321894647.75</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>505672.03157746251</v>
       </c>
       <c r="R39">
@@ -4593,23 +4593,23 @@
         <v>8427.8671929577085</v>
       </c>
       <c r="S39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>351.16113303990454</v>
       </c>
       <c r="T39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.96208529599973847</v>
       </c>
       <c r="V39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>438249.09403380082</v>
       </c>
       <c r="W39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>842786.71929577086</v>
       </c>
       <c r="X39">
-        <f>R39 *200</f>
+        <f t="shared" si="1"/>
         <v>1685573.4385915417</v>
       </c>
     </row>
@@ -4618,7 +4618,7 @@
         <v>25</v>
       </c>
       <c r="O40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>625</v>
       </c>
       <c r="P40">
@@ -4626,7 +4626,7 @@
         <v>289014709125073.56</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4816911.8187512262</v>
       </c>
       <c r="R40">
@@ -4634,23 +4634,23 @@
         <v>80281.863645853766</v>
       </c>
       <c r="S40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3345.0776519105734</v>
       </c>
       <c r="T40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.1645963066043112</v>
       </c>
       <c r="V40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4174656.9095843956</v>
       </c>
       <c r="W40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8028186.3645853763</v>
       </c>
       <c r="X40">
-        <f>R40 *200</f>
+        <f t="shared" si="1"/>
         <v>16056372.729170753</v>
       </c>
     </row>
@@ -4659,15 +4659,15 @@
         <v>26</v>
       </c>
       <c r="O41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>676</v>
       </c>
       <c r="P41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3018386160045016.5</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>50306436.000750273</v>
       </c>
       <c r="R41">
@@ -4675,23 +4675,23 @@
         <v>838440.60001250461</v>
       </c>
       <c r="S41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>34935.025000521026</v>
       </c>
       <c r="T41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>95.71239726170144</v>
       </c>
       <c r="V41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>43598911.200650238</v>
       </c>
       <c r="W41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>83844060.001250461</v>
       </c>
       <c r="X41">
-        <f>R41 *200</f>
+        <f t="shared" si="1"/>
         <v>167688120.00250092</v>
       </c>
     </row>
@@ -4700,15 +4700,15 @@
         <v>27</v>
       </c>
       <c r="O42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>729</v>
       </c>
       <c r="P42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4560876470885548E+16</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>576014607.84809244</v>
       </c>
       <c r="R42">
@@ -4716,11 +4716,11 @@
         <v>9600243.4641348738</v>
       </c>
       <c r="S42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>400010.14433895308</v>
       </c>
       <c r="T42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1095.9182036683646</v>
       </c>
     </row>
@@ -4729,15 +4729,15 @@
         <v>28</v>
       </c>
       <c r="O43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>784</v>
       </c>
       <c r="P43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.3386017486589491E+17</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7231002914.4315815</v>
       </c>
       <c r="R43">
@@ -4745,11 +4745,11 @@
         <v>120516715.24052636</v>
       </c>
       <c r="S43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5021529.8016885985</v>
       </c>
       <c r="T43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13757.615895037256</v>
       </c>
     </row>
@@ -4758,7 +4758,7 @@
         <v>29</v>
       </c>
       <c r="O44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>841</v>
       </c>
       <c r="P44">
@@ -4766,7 +4766,7 @@
         <v>5.97131413012126E+18</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>99521902168.687668</v>
       </c>
       <c r="R44">
@@ -4774,11 +4774,11 @@
         <v>1658698369.4781277</v>
       </c>
       <c r="S44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>69112432.06158866</v>
       </c>
       <c r="T44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>189349.12893585933</v>
       </c>
     </row>
@@ -4787,15 +4787,15 @@
         <v>30</v>
       </c>
       <c r="O45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>900</v>
       </c>
       <c r="P45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.0104222262885646E+19</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1501737037714.7607</v>
       </c>
       <c r="R45">
@@ -4803,11 +4803,11 @@
         <v>25028950628.579346</v>
       </c>
       <c r="S45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1042872942.8574728</v>
       </c>
       <c r="T45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2857186.1448149937</v>
       </c>
     </row>
@@ -4816,15 +4816,15 @@
         <v>31</v>
       </c>
       <c r="O46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>961</v>
       </c>
       <c r="P46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.490649224944159E+21</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24844153749069.316</v>
       </c>
       <c r="R46">
@@ -4832,11 +4832,11 @@
         <v>414069229151.15527</v>
       </c>
       <c r="S46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17252884547.964802</v>
       </c>
       <c r="T46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>47268176.843739182</v>
       </c>
     </row>
@@ -4845,15 +4845,15 @@
         <v>32</v>
       </c>
       <c r="O47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1024</v>
       </c>
       <c r="P47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.7037147304012666E+22</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>450619121733544.44</v>
       </c>
       <c r="R47">
@@ -4861,11 +4861,11 @@
         <v>7510318695559.0742</v>
       </c>
       <c r="S47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>312929945648.29474</v>
       </c>
       <c r="T47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>857342316.84464312</v>
       </c>
     </row>
@@ -4874,15 +4874,15 @@
         <v>50</v>
       </c>
       <c r="O48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
       <c r="P48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.2950500441646779E+51</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3825083406941131E+44</v>
       </c>
       <c r="R48">
@@ -4890,11 +4890,11 @@
         <v>2.3041805678235216E+42</v>
       </c>
       <c r="S48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.6007523659313406E+40</v>
       </c>
       <c r="T48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.630343113953792E+38</v>
       </c>
     </row>
@@ -4903,15 +4903,15 @@
         <v>100</v>
       </c>
       <c r="O49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10000</v>
       </c>
       <c r="P49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.6287928627313866E+201</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.3813214378856448E+193</v>
       </c>
       <c r="R49">
@@ -4919,11 +4919,11 @@
         <v>1.5635535729809406E+192</v>
       </c>
       <c r="S49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.5148065540872527E+190</v>
       </c>
       <c r="T49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7848785079691103E+188</v>
       </c>
     </row>

</xml_diff>